<commit_message>
paket-soal: download template soal
</commit_message>
<xml_diff>
--- a/public/Template/test.xlsx
+++ b/public/Template/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laravel\niagacoding\Try-Out-App\public\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821766A8-1CD8-4092-964A-C07729DAFBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3BC0-1AEA-4D80-8444-612D5BEF5192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,10 +91,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +413,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,53 +443,53 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>